<commit_message>
replace testing doc with updated
</commit_message>
<xml_diff>
--- a/docs/testing/Testing MP1.xlsx
+++ b/docs/testing/Testing MP1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanya\OneDrive\Documents\CODING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanya\OneDrive\Documents\CODING\MP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9B1A44-3E2A-4306-B15A-52AE9B3B82AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BAA890-8CC6-49B3-BCAD-73F1C02284F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="75" windowWidth="27135" windowHeight="15075" xr2:uid="{AEC060EB-3314-4159-9268-8C5C3FC6A3E7}"/>
+    <workbookView xWindow="615" yWindow="1065" windowWidth="27135" windowHeight="15075" xr2:uid="{AEC060EB-3314-4159-9268-8C5C3FC6A3E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="185">
   <si>
     <t>PASS/FAIL</t>
   </si>
@@ -1307,6 +1307,31 @@
   </si>
   <si>
     <t>Fixed.</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>Testing 404 page</t>
+  </si>
+  <si>
+    <t>Typing an incorrect address bring you to a customer 404 page with a link back to home</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Open site in browser
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>• Type incorrect address into address bar
+• Hit enter</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1728,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D5D565-BF97-4AC8-B2CD-BD1689AF0EF9}">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,77 +2359,74 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="5" t="s">
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="7"/>
+      <c r="B32" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>81</v>
@@ -2413,44 +2435,44 @@
         <v>48</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>81</v>
@@ -2459,44 +2481,44 @@
         <v>49</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>170</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>81</v>
@@ -2505,44 +2527,44 @@
         <v>78</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>82</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>81</v>
@@ -2551,86 +2573,86 @@
         <v>79</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="D41" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
-      <c r="B42" s="5" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
+      <c r="B43" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>86</v>
@@ -2639,18 +2661,21 @@
         <v>85</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>86</v>
@@ -2659,21 +2684,18 @@
         <v>85</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>86</v>
@@ -2682,18 +2704,21 @@
         <v>85</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>86</v>
@@ -2702,21 +2727,18 @@
         <v>85</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>88</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>86</v>
@@ -2725,18 +2747,21 @@
         <v>85</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>141</v>
+      <c r="A50" t="s">
+        <v>140</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>86</v>
@@ -2745,21 +2770,18 @@
         <v>85</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>86</v>
@@ -2768,85 +2790,85 @@
         <v>85</v>
       </c>
       <c r="E51" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A53" s="7"/>
-      <c r="B53" s="5" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A54" s="7"/>
+      <c r="B54" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B55" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D55" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G55" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>147</v>
@@ -2855,21 +2877,21 @@
         <v>146</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>147</v>
@@ -2878,21 +2900,21 @@
         <v>146</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>147</v>
@@ -2901,21 +2923,21 @@
         <v>146</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>147</v>
@@ -2924,21 +2946,21 @@
         <v>146</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>147</v>
@@ -2947,21 +2969,21 @@
         <v>146</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>147</v>
@@ -2975,39 +2997,53 @@
       <c r="F61" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G61" s="1"/>
+      <c r="G61" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>147</v>
       </c>
       <c r="D62" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G62" s="1" t="s">
+      <c r="F63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -3054,6 +3090,15 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>